<commit_message>
A few more true labels
</commit_message>
<xml_diff>
--- a/research/document_types/ground_truth.xlsx
+++ b/research/document_types/ground_truth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vita/Code/demokratis/demokratis-ml/research/document_types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC94AC6-2771-0046-B2DE-7C57FDEC3092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A222A08-FC81-BF4F-87BB-293D321F167E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{B5B270AF-2AEF-0544-AE5F-781A826AE502}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="205">
   <si>
     <t>document_id</t>
   </si>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2181,7 +2181,9 @@
       <c r="C76" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D76" s="2"/>
+      <c r="D76" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2194,7 +2196,9 @@
       <c r="C77" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="2"/>
+      <c r="D77" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2246,7 +2250,9 @@
       <c r="C81" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D81" s="2"/>
+      <c r="D81" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2259,7 +2265,9 @@
       <c r="C82" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D82" s="2"/>
+      <c r="D82" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E82" s="2"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2298,7 +2306,9 @@
       <c r="C85" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D85" s="2"/>
+      <c r="D85" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E85" s="2"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2324,7 +2334,9 @@
       <c r="C87" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D87" s="2"/>
+      <c r="D87" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2337,7 +2349,9 @@
       <c r="C88" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D88" s="2"/>
+      <c r="D88" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2350,7 +2364,9 @@
       <c r="C89" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D89" s="2"/>
+      <c r="D89" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2376,7 +2392,9 @@
       <c r="C91" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D91" s="2"/>
+      <c r="D91" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2389,7 +2407,9 @@
       <c r="C92" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D92" s="2"/>
+      <c r="D92" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E92" s="2"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2402,7 +2422,9 @@
       <c r="C93" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D93" s="2"/>
+      <c r="D93" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2415,7 +2437,9 @@
       <c r="C94" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D94" s="2"/>
+      <c r="D94" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E94" s="2"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2428,7 +2452,9 @@
       <c r="C95" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D95" s="2"/>
+      <c r="D95" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E95" s="2"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2506,108 +2532,110 @@
       <c r="C101" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D101" s="2"/>
+      <c r="D101" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E101" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{86B3A93D-6441-1843-B852-E409C8119A63}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{3DBA9549-28A2-204B-9618-FA06E0D6D7F5}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{F2AD1E63-34BC-8D40-A2DF-44E809DB579D}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{410761D6-C5AC-5742-9FFE-603B355C6642}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{D743E019-6F39-3742-B113-910E3F3F33A1}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{868DAC51-40F7-9041-8679-52A60E2538CD}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{D6D175E0-32F7-5542-8ABE-450CF49A14D5}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{2EC09173-6E1E-BA4E-8DE2-C1C2B53EEAF6}"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://www.notes.zh.ch/sk/VNL/vnl.nsf/vw-alldocuments/78C5643FF13097C6C12582AC002F00FD/$File/EnerG-Aend MuKEn2014 Vern18 2018-04-12 Versandexemplar-Beilage.pdf" xr:uid="{8318992A-2C1C-314B-88A9-53721F015149}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{8FEBF397-1482-B340-9C82-583183A09ABA}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{3577460C-EE52-034B-823E-FE53DE0890AF}"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://www.sg.ch/news/sgch_allgemein/2019/05/vi--nachtrag-vom-energiegesetz/_jcr_content/Par/sgch_downloadlist/DownloadListPar/sgch_download_copy_1776316844.ocFile/VI. Nachtrag Energiegesetz.pdf" xr:uid="{A7B445DE-4A1B-B445-B793-AD84211E8CBC}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{7EBF87A5-3FB1-0E4E-8928-8FD892EF8A9B}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{42B579DB-99A9-EC41-96B9-79B30171F6CA}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{AF0B823C-4A08-B24F-B7EB-FBE1DAB452F4}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{7C3CBEAA-B49C-7441-B126-6B79942DE340}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{94F90466-EB84-FD46-8961-938D94C495EA}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{CA563E50-706E-FB4E-A3D1-74A1E6E14CD8}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{7641ADED-116B-884B-91D5-96FC58AFCD8E}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{0A90FF61-68C7-EB42-88C4-656EEB6630AB}"/>
-    <hyperlink ref="B22" r:id="rId21" xr:uid="{4B589673-45ED-E54E-89E4-0357A5CF3E6D}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{F5C5680A-97C6-814B-91E4-B18CC2580752}"/>
-    <hyperlink ref="B24" r:id="rId23" xr:uid="{06CF2C5F-D6EE-B247-B5F3-62904613694E}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{FE8F0721-01CD-A34F-BD8A-1CEE8AE9F2E9}"/>
-    <hyperlink ref="B26" r:id="rId25" xr:uid="{CAEF2C6F-1CB3-4F4F-A81F-C6ED4C209661}"/>
-    <hyperlink ref="B27" r:id="rId26" xr:uid="{BA464509-5AE0-F44E-9D20-BA092F2FCAB1}"/>
-    <hyperlink ref="B28" r:id="rId27" xr:uid="{ECA2D59A-8934-0849-85BF-14F4471E1342}"/>
-    <hyperlink ref="B29" r:id="rId28" xr:uid="{CB153200-9CD5-384F-B2B7-086A21C22630}"/>
-    <hyperlink ref="B30" r:id="rId29" xr:uid="{E3F021B6-8A0A-2E45-98CD-3AF462141CDC}"/>
-    <hyperlink ref="B31" r:id="rId30" xr:uid="{2BE7DB69-E02B-C84A-8EE0-DE9329ECB9D8}"/>
-    <hyperlink ref="B32" r:id="rId31" xr:uid="{733C9A08-3D54-4744-8919-090ACCFECE30}"/>
-    <hyperlink ref="B33" r:id="rId32" xr:uid="{18EC1D5A-1251-584B-B276-703150656A6A}"/>
-    <hyperlink ref="B34" r:id="rId33" xr:uid="{8901D3F5-58EA-B245-AF5C-6CD36A9B3C0C}"/>
-    <hyperlink ref="B35" r:id="rId34" xr:uid="{072BD2B4-FC3E-6D44-AA3E-4FC0FCC0D308}"/>
-    <hyperlink ref="B36" r:id="rId35" xr:uid="{CB9E06DE-2401-4145-9EA0-DF6EE48AC18C}"/>
-    <hyperlink ref="B37" r:id="rId36" xr:uid="{A3E2FD4A-9710-CD46-AFAF-7DC954F85541}"/>
-    <hyperlink ref="B38" r:id="rId37" xr:uid="{D810187F-EC96-7147-9B3F-D47F4D629E6A}"/>
-    <hyperlink ref="B40" r:id="rId38" display="https://www.gl.ch/public/upload/assets/42746/Bericht und Antrag an LR.pdf?fp=1" xr:uid="{74156008-00E9-2C47-AE46-C3B0CB832B6A}"/>
-    <hyperlink ref="B41" r:id="rId39" xr:uid="{2AC9E69D-2FD2-B642-8CDD-D4F2866A2BFC}"/>
-    <hyperlink ref="B42" r:id="rId40" xr:uid="{CC1F1B2F-9041-A240-9416-3128DC10BF86}"/>
-    <hyperlink ref="B43" r:id="rId41" xr:uid="{97D7DB77-DE4F-E94C-B272-7501B4C76812}"/>
-    <hyperlink ref="B44" r:id="rId42" xr:uid="{3EFBFADF-E7F7-9C46-AD6E-5BADFA41B1BA}"/>
-    <hyperlink ref="B45" r:id="rId43" xr:uid="{86E1CF35-4FE0-1E40-8D76-06B8F381B1A5}"/>
-    <hyperlink ref="B46" r:id="rId44" xr:uid="{A8B28A86-6088-3741-9AA2-4C8F6CD377FD}"/>
-    <hyperlink ref="B47" r:id="rId45" xr:uid="{C9FB0756-F279-FA4F-9308-DC06D68ABC55}"/>
-    <hyperlink ref="B48" r:id="rId46" xr:uid="{5380134C-9940-EA45-B6D1-B7132784E9BE}"/>
-    <hyperlink ref="B49" r:id="rId47" xr:uid="{283FE271-F697-CA4B-878A-C3A2FAF13BDB}"/>
-    <hyperlink ref="B50" r:id="rId48" xr:uid="{5CC15394-2F77-1947-94C1-764AA0F1D106}"/>
-    <hyperlink ref="B51" r:id="rId49" display="https://zg.ch/dam/jcr:95397bc7-9729-4e66-9c3c-e82933beb56e/Antwortformular_Vernehmlassung betreffend %C3%84nderung der Verordnung zum Einf%C3%BChrungsgesetz zum Bundesgesetz %C3%BCber die Familienzulage.pdf" xr:uid="{33A40DD8-3620-E848-A6AE-AB6DDE38453F}"/>
-    <hyperlink ref="B52" r:id="rId50" xr:uid="{AB1B6B2D-7C73-174A-9EF3-A71D8CE7B296}"/>
-    <hyperlink ref="B53" r:id="rId51" xr:uid="{B90618C9-FA81-5B41-821C-932C35446E2A}"/>
-    <hyperlink ref="B54" r:id="rId52" xr:uid="{29FE8386-6506-1F41-A374-3EE0AA227170}"/>
-    <hyperlink ref="B55" r:id="rId53" xr:uid="{A0C80167-FABA-FE4E-BE92-4BF74F2AB660}"/>
-    <hyperlink ref="B56" r:id="rId54" xr:uid="{85DD5BF5-B492-3C48-996A-B9D8B0CA54B8}"/>
-    <hyperlink ref="B57" r:id="rId55" display="https://www.notes.zh.ch/sk/VNL/vnl.nsf/vw-alldocuments/7FE8032D1A779F34C125814F0036EA1C/$File/RRB Gesetzesanpassungen GesG_EpG.pdf" xr:uid="{79569A6F-005A-EE4C-B37F-4B9BAC0BAF14}"/>
-    <hyperlink ref="B58" r:id="rId56" xr:uid="{584606E1-6F23-4042-978C-6A62B3B389C3}"/>
-    <hyperlink ref="B59" r:id="rId57" display="https://vernehmlassungen.tg.ch/public/upload/assets/113256/Entwurf_ Gesetz_Teilrevision_Netzbeschluss.pdf?fp=1620020976371" xr:uid="{1EAC25F4-E02B-C046-ADF5-C0160E924474}"/>
-    <hyperlink ref="B60" r:id="rId58" xr:uid="{5AEAD75C-F673-4C4F-9919-6B0C379FDD6E}"/>
-    <hyperlink ref="B61" r:id="rId59" xr:uid="{028C11C5-F180-6C4B-8EE6-02B6782C9479}"/>
-    <hyperlink ref="B62" r:id="rId60" xr:uid="{24AE5AD3-9D8E-AA42-B627-EF2B83B6215A}"/>
-    <hyperlink ref="B63" r:id="rId61" xr:uid="{19385724-43F2-E946-A96B-92E9DA67D587}"/>
-    <hyperlink ref="B64" r:id="rId62" xr:uid="{9C805B04-7B88-6E4E-83DD-84E26F051E42}"/>
-    <hyperlink ref="B65" r:id="rId63" xr:uid="{29A9E675-A7E7-134F-BF66-BE04DD933007}"/>
-    <hyperlink ref="B66" r:id="rId64" display="https://zg.ch/dam/jcr:c2f415ec-de6e-4145-9149-697390fe4452/Entwurf des totalrevidierten Gesetzes ueber Ausbildungsbeitraege (ID 2565).pdf" xr:uid="{1FDC866C-41AE-404E-BF5E-3A2FEC326995}"/>
-    <hyperlink ref="B67" r:id="rId65" display="https://www.gl.ch/public/upload/assets/35187/Antrag an den LR.pdf?fp=1" xr:uid="{5ABC43F8-6850-0F41-96E6-E30D884323C4}"/>
-    <hyperlink ref="B69" r:id="rId66" xr:uid="{26F9B431-91F4-9645-8387-B58D242EADFF}"/>
-    <hyperlink ref="B70" r:id="rId67" display="https://www.notes.zh.ch/sk/VNL/vnl.nsf/vw-alldocuments/699F95F30D35934CC1257619003B33E6/$File/Medical Board Medienmitteilung.pdf" xr:uid="{5F3D36A8-240B-FC47-B79D-A798847AEE22}"/>
-    <hyperlink ref="B71" r:id="rId68" xr:uid="{D57D3B31-F310-8448-BBA3-498A358033AA}"/>
-    <hyperlink ref="B72" r:id="rId69" xr:uid="{A5CC6B24-F0A5-2541-B12E-6EF5D88D07DE}"/>
-    <hyperlink ref="B73" r:id="rId70" xr:uid="{76592814-C32C-9D4B-A34E-B3D5331BA8B7}"/>
-    <hyperlink ref="B74" r:id="rId71" xr:uid="{C809AB33-EB06-794D-A23B-45591B3785B0}"/>
-    <hyperlink ref="B75" r:id="rId72" xr:uid="{A5936FCB-CD91-9B40-A625-5D1E884132D1}"/>
-    <hyperlink ref="B76" r:id="rId73" xr:uid="{A72DA2EA-9007-1349-B068-48CEBECB8251}"/>
-    <hyperlink ref="B77" r:id="rId74" xr:uid="{568B6C4F-05A1-2344-887B-A6108C1900B4}"/>
-    <hyperlink ref="B78" r:id="rId75" xr:uid="{03DCC453-0435-A941-9285-1F0550BEB4D3}"/>
-    <hyperlink ref="B79" r:id="rId76" xr:uid="{4351AECB-5CB0-3742-86D3-6D191607E4AC}"/>
-    <hyperlink ref="B80" r:id="rId77" xr:uid="{D588FD4B-A78E-CC42-9A55-528535C38A79}"/>
-    <hyperlink ref="B81" r:id="rId78" xr:uid="{68425207-916D-D24F-A142-CC3BAE858D0F}"/>
-    <hyperlink ref="B82" r:id="rId79" xr:uid="{F8CC1407-ABB1-774C-989F-451B7DB71E4D}"/>
-    <hyperlink ref="B83" r:id="rId80" xr:uid="{33FCEB93-40D0-584E-A60D-A876A7E341A4}"/>
-    <hyperlink ref="B84" r:id="rId81" xr:uid="{F1CCEC08-589F-1344-8C45-52BFAE8214D5}"/>
-    <hyperlink ref="B85" r:id="rId82" xr:uid="{FDA40FD9-C7A8-AC47-86BB-2B427256550B}"/>
-    <hyperlink ref="B86" r:id="rId83" xr:uid="{ABFBED2B-A8EB-AF4E-A7BA-74F286C7EC1B}"/>
-    <hyperlink ref="B87" r:id="rId84" xr:uid="{09AC6A82-094F-B748-91FE-6C06F4D68A57}"/>
-    <hyperlink ref="B88" r:id="rId85" xr:uid="{B20C0EC8-4ECE-4D41-8579-F59B7B3BA404}"/>
-    <hyperlink ref="B89" r:id="rId86" xr:uid="{D321D8B1-2183-1C4E-8D81-D8F0F256E1BA}"/>
-    <hyperlink ref="B90" r:id="rId87" xr:uid="{CD938252-3123-5845-A62D-1AB952CDB97D}"/>
-    <hyperlink ref="B91" r:id="rId88" xr:uid="{0A396CEC-C747-C04D-9F9D-380286382B04}"/>
-    <hyperlink ref="B92" r:id="rId89" xr:uid="{A9280AB5-8BB1-0748-A99B-BE05BBE29711}"/>
-    <hyperlink ref="B93" r:id="rId90" display="https://www.gl.ch/public/upload/assets/54745/Einladung zur Vernehmlassung.pdf?fp=1" xr:uid="{DFEC4B01-07AF-2D4A-90AA-736CE553CD99}"/>
-    <hyperlink ref="B94" r:id="rId91" xr:uid="{ED984AF4-9CC6-BD41-96AB-532358B234C8}"/>
-    <hyperlink ref="B95" r:id="rId92" xr:uid="{2E10A7FF-E751-2A41-87A8-A8B3188C7087}"/>
-    <hyperlink ref="B97" r:id="rId93" xr:uid="{F27E3DC4-7C3E-D841-BC43-1581D6A0969A}"/>
-    <hyperlink ref="B98" r:id="rId94" xr:uid="{24B4DAE0-2336-7A4A-8091-74289759AD1C}"/>
-    <hyperlink ref="B99" r:id="rId95" xr:uid="{420263B5-CFCE-DF46-981F-FACA46666C2A}"/>
-    <hyperlink ref="B100" r:id="rId96" xr:uid="{DC1A90E5-EA3C-1844-90C3-F1768489483E}"/>
-    <hyperlink ref="B101" r:id="rId97" display="https://www.notes.zh.ch/sk/VNL/vnl.nsf/vw-alldocuments/0171AD859145F8B0C1258BDC0045AA29/$File/Antrag RR KR-Nr. 61a2021.pdf" xr:uid="{9B2C4EFF-6021-D848-B5AE-CBA4B82BD7E7}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{EDC24CD6-3D86-4C48-8B80-3FE3F78F71C2}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8E8AFFCF-D6CF-9A40-9347-08CA83C3A88F}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{3338E588-7481-8E4C-B404-0F3DA573EC41}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{F4B775BB-E5D5-4949-BD6C-93B1F64CEE3B}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{34F71093-5C84-0945-83B2-24FDE78E2D73}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{D7B82C26-363E-F045-B972-9BE20D59A6E9}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{C031EAF1-D05C-D946-8843-F8FA188DE1AC}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{6200CCE6-6969-1548-9ECF-8BADF90287B2}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://www.notes.zh.ch/sk/VNL/vnl.nsf/vw-alldocuments/78C5643FF13097C6C12582AC002F00FD/$File/EnerG-Aend MuKEn2014 Vern18 2018-04-12 Versandexemplar-Beilage.pdf" xr:uid="{C35D42F9-0933-174C-9CBA-CA9162C47AC0}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{AFC2D2BB-0272-8548-92D6-05A5E910AC0F}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{9AD6413B-6BCD-5742-81A5-24D8E2614B7D}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://www.sg.ch/news/sgch_allgemein/2019/05/vi--nachtrag-vom-energiegesetz/_jcr_content/Par/sgch_downloadlist/DownloadListPar/sgch_download_copy_1776316844.ocFile/VI. Nachtrag Energiegesetz.pdf" xr:uid="{4D92DE27-2D9F-2E47-9B05-B857ADD1D275}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{2174B8F7-1C0E-784A-93D5-A048E87901E6}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{28565C33-38A6-FD4E-8B65-D13142D0D303}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{66E9C302-157D-CC42-9C49-AE1DD0117037}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{C088FD7A-0DBC-7147-85FF-52558C7BC025}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{1A120F43-62D1-314F-8B02-1DE2651E5C5C}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{8D6ED970-0066-3947-BA76-11331E0DEC97}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{6195343C-3E86-3646-9153-54B08E78F672}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{500BA2B4-3C44-2A4A-9940-ECD4CFE5E89F}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{8B0F237C-303B-2240-9B02-7220798B3693}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{90BAC36C-0304-C14E-9707-B9C5EAF76705}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{64F7778A-1FD6-8140-B43E-C472CD961DE5}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{16592ACF-5EA8-A94E-9A5F-F01D2CCB2A8A}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{B9217CF6-6F1C-E34A-8501-68364937153B}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{1AC18E04-DD6D-F74B-A107-7CD1AB178131}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{7875FEE6-50BF-C148-984E-2A8C5860BA26}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{47466C0E-3360-4B4D-B57C-13C11C4F3FEE}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{7DAA3528-81DB-B54D-B047-43CF52F39707}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{C217E41C-745B-7C49-BBAB-E6530A19EC0E}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{4F2224A3-4E38-834D-A14B-E81A1B23AE06}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{E203FB95-2396-DE4C-B7E7-3D7743A44120}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{274F4E19-496B-A84F-819A-B2119CCFA186}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{A167C4DF-867E-4C48-B64B-BC68382D2041}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{F6486301-8549-3242-BA6A-1448DA4F3CF6}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{4C564EF2-249F-0D43-8B61-2FE54EDDE7F0}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{5002EC5A-E17D-F44E-98C0-7EB1BEA06B9B}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://www.gl.ch/public/upload/assets/42746/Bericht und Antrag an LR.pdf?fp=1" xr:uid="{75D615DF-2EA5-8146-B406-8A67AD3AFA27}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{26A6D095-8157-924A-830D-8AB16FE0B06D}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{AADB8104-A222-F54A-9544-DCACB28FF773}"/>
+    <hyperlink ref="B43" r:id="rId41" xr:uid="{00E72B3F-F4CD-AE4C-A5C4-104B65E7381B}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{01209E9D-0447-414B-9CA9-B50CE4ED6CA2}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{AEB9C4B2-5FFE-1A41-ACCA-5F4382854234}"/>
+    <hyperlink ref="B46" r:id="rId44" xr:uid="{F82EBEEF-D19B-3048-AA08-DC328247407E}"/>
+    <hyperlink ref="B47" r:id="rId45" xr:uid="{75B5A4B2-78DB-6A49-AE89-A70856F3CB5F}"/>
+    <hyperlink ref="B48" r:id="rId46" xr:uid="{F4E654E1-E8E9-BB4A-85E6-B1505A11CAFC}"/>
+    <hyperlink ref="B49" r:id="rId47" xr:uid="{F412F401-2838-7048-9B5C-B8423E72E3FB}"/>
+    <hyperlink ref="B50" r:id="rId48" xr:uid="{2805EB01-5C2A-6747-81FC-3C97351696F0}"/>
+    <hyperlink ref="B51" r:id="rId49" display="https://zg.ch/dam/jcr:95397bc7-9729-4e66-9c3c-e82933beb56e/Antwortformular_Vernehmlassung betreffend %C3%84nderung der Verordnung zum Einf%C3%BChrungsgesetz zum Bundesgesetz %C3%BCber die Familienzulage.pdf" xr:uid="{E6E5ECBA-D9AB-C547-8415-73F73D671011}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{CBA99F26-1AE3-824B-BDD2-D892E3A7E4E5}"/>
+    <hyperlink ref="B53" r:id="rId51" xr:uid="{74C0B64B-000C-014F-B39B-6EFDF4EA5DAE}"/>
+    <hyperlink ref="B54" r:id="rId52" xr:uid="{C19AF4AD-80DB-6D46-A3F5-C79D2E02249F}"/>
+    <hyperlink ref="B55" r:id="rId53" xr:uid="{CDB483B3-B9C7-0F45-A35B-5991C4DA3E3C}"/>
+    <hyperlink ref="B56" r:id="rId54" xr:uid="{709AE957-089F-B643-868B-232EF832B549}"/>
+    <hyperlink ref="B57" r:id="rId55" display="https://www.notes.zh.ch/sk/VNL/vnl.nsf/vw-alldocuments/7FE8032D1A779F34C125814F0036EA1C/$File/RRB Gesetzesanpassungen GesG_EpG.pdf" xr:uid="{1608493F-1BD8-3B4F-9CBD-6457007337DC}"/>
+    <hyperlink ref="B58" r:id="rId56" xr:uid="{5428CF9B-A9FE-A548-9A52-F95DE8A8AA22}"/>
+    <hyperlink ref="B59" r:id="rId57" display="https://vernehmlassungen.tg.ch/public/upload/assets/113256/Entwurf_ Gesetz_Teilrevision_Netzbeschluss.pdf?fp=1620020976371" xr:uid="{142EE557-1679-4348-9BCE-2B6AC9B720F8}"/>
+    <hyperlink ref="B60" r:id="rId58" xr:uid="{C46867AC-F124-0D44-A96C-53DEE8BB15DF}"/>
+    <hyperlink ref="B61" r:id="rId59" xr:uid="{7C7412CE-8356-8B43-AE3D-38AE20C74880}"/>
+    <hyperlink ref="B62" r:id="rId60" xr:uid="{2BDDAF70-BF8D-2A4A-AD4E-CA0605E35AD1}"/>
+    <hyperlink ref="B63" r:id="rId61" xr:uid="{A612B8FE-FDA6-0D42-9093-B155AAFA0C66}"/>
+    <hyperlink ref="B64" r:id="rId62" xr:uid="{981E7916-91BC-0540-A93E-D96A059C73E7}"/>
+    <hyperlink ref="B65" r:id="rId63" xr:uid="{82660A73-B9BE-9A48-9530-DF48F666E8D1}"/>
+    <hyperlink ref="B66" r:id="rId64" display="https://zg.ch/dam/jcr:c2f415ec-de6e-4145-9149-697390fe4452/Entwurf des totalrevidierten Gesetzes ueber Ausbildungsbeitraege (ID 2565).pdf" xr:uid="{312F7A61-4BE1-7C45-A941-3693C9F96ABA}"/>
+    <hyperlink ref="B67" r:id="rId65" display="https://www.gl.ch/public/upload/assets/35187/Antrag an den LR.pdf?fp=1" xr:uid="{0A2542C6-9A3A-0D47-9792-1DDD55ACCFD2}"/>
+    <hyperlink ref="B69" r:id="rId66" xr:uid="{474A21BA-BC8A-1144-8181-01ADBC8BD72E}"/>
+    <hyperlink ref="B70" r:id="rId67" display="https://www.notes.zh.ch/sk/VNL/vnl.nsf/vw-alldocuments/699F95F30D35934CC1257619003B33E6/$File/Medical Board Medienmitteilung.pdf" xr:uid="{3DB82462-4F9B-EC4C-A3D9-7197313B9EB1}"/>
+    <hyperlink ref="B71" r:id="rId68" xr:uid="{564446EF-18DA-9B41-8F07-F0DAAE48F861}"/>
+    <hyperlink ref="B72" r:id="rId69" xr:uid="{88375FB0-CEA0-1B4E-9DED-5D07FE9EFFF9}"/>
+    <hyperlink ref="B73" r:id="rId70" xr:uid="{58C22D9A-E068-234B-9A00-F7828B4FAF9D}"/>
+    <hyperlink ref="B74" r:id="rId71" xr:uid="{0D68BCF3-E242-EE4E-AD23-7A6E97C89A19}"/>
+    <hyperlink ref="B75" r:id="rId72" xr:uid="{D804B205-5977-C049-B81A-4FE4657082BA}"/>
+    <hyperlink ref="B76" r:id="rId73" xr:uid="{57886D55-F727-3246-8075-705594E26628}"/>
+    <hyperlink ref="B77" r:id="rId74" xr:uid="{F215D2A3-6577-114F-9F75-782792A92CDA}"/>
+    <hyperlink ref="B78" r:id="rId75" xr:uid="{2AA77B39-71A6-2A4A-8D8E-CF99D0D63913}"/>
+    <hyperlink ref="B79" r:id="rId76" xr:uid="{9939FE30-CA26-2041-870E-470FE37BA99C}"/>
+    <hyperlink ref="B80" r:id="rId77" xr:uid="{3250339E-54BE-744D-BC2F-9B8BEF9686BC}"/>
+    <hyperlink ref="B81" r:id="rId78" xr:uid="{DB8B140E-8CAA-5D4C-84AC-12728EA20038}"/>
+    <hyperlink ref="B82" r:id="rId79" xr:uid="{71713C9A-6ED7-FC47-BC11-085E668CD925}"/>
+    <hyperlink ref="B83" r:id="rId80" xr:uid="{C2D2A739-79B3-254F-B410-DF3B65A722C3}"/>
+    <hyperlink ref="B84" r:id="rId81" xr:uid="{1F9813D2-09E5-DD41-8A6D-39B6F5D69CAA}"/>
+    <hyperlink ref="B85" r:id="rId82" xr:uid="{B510FD47-7561-D046-981D-53BAF222296A}"/>
+    <hyperlink ref="B86" r:id="rId83" xr:uid="{402F03D3-FB4D-3D40-A05C-0FD06029FBA6}"/>
+    <hyperlink ref="B87" r:id="rId84" xr:uid="{7CB21980-F73A-914A-8F03-09F777BE6227}"/>
+    <hyperlink ref="B88" r:id="rId85" xr:uid="{B206218D-175C-6348-A7EF-9D2182B70B8C}"/>
+    <hyperlink ref="B89" r:id="rId86" xr:uid="{3B2FC341-F960-1146-A087-C942AF6825DC}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{5D376F1E-8BAE-714C-B69C-37B1D3D1134D}"/>
+    <hyperlink ref="B91" r:id="rId88" xr:uid="{BF54381C-F110-FA40-8454-49CE6773353D}"/>
+    <hyperlink ref="B92" r:id="rId89" xr:uid="{66ADF74F-0F31-FA4A-845C-DC486AB38380}"/>
+    <hyperlink ref="B93" r:id="rId90" display="https://www.gl.ch/public/upload/assets/54745/Einladung zur Vernehmlassung.pdf?fp=1" xr:uid="{1B815B07-0D67-D04C-B736-672FE8522033}"/>
+    <hyperlink ref="B94" r:id="rId91" xr:uid="{D2C15B68-B955-2342-952C-A1E616950C01}"/>
+    <hyperlink ref="B95" r:id="rId92" xr:uid="{6C37B1A1-9CD4-2642-A8C1-3E33CCC5CF2B}"/>
+    <hyperlink ref="B97" r:id="rId93" xr:uid="{59B64E60-19EF-3F46-94B8-24243F2D53DC}"/>
+    <hyperlink ref="B98" r:id="rId94" xr:uid="{FEB422B5-9A16-6A41-8F59-15449279DE78}"/>
+    <hyperlink ref="B99" r:id="rId95" xr:uid="{2E794BF9-2FDB-0047-83E8-AA21FDF933E2}"/>
+    <hyperlink ref="B100" r:id="rId96" xr:uid="{672D6C4B-B203-A14B-9B43-C6F1FDBDB7C1}"/>
+    <hyperlink ref="B101" r:id="rId97" display="https://www.notes.zh.ch/sk/VNL/vnl.nsf/vw-alldocuments/0171AD859145F8B0C1258BDC0045AA29/$File/Antrag RR KR-Nr. 61a2021.pdf" xr:uid="{452380C1-F45F-4C44-B28A-6351A3DAF8EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update the ground_truth table - fix some incorrect manual labels
</commit_message>
<xml_diff>
--- a/research/document_types/ground_truth.xlsx
+++ b/research/document_types/ground_truth.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vita/Code/demokratis/demokratis-ml/research/document_types/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9F6DC8-8F1F-8D45-BCDE-7229FA911F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="36080" yWindow="500" windowWidth="24060" windowHeight="33340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="390">
   <si>
     <t>document_id</t>
   </si>
@@ -1175,31 +1184,49 @@
   </si>
   <si>
     <t>Majorz Übersicht</t>
+  </si>
+  <si>
+    <t>OPINION</t>
+  </si>
+  <si>
+    <t>DECISION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1207,42 +1234,46 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1432,26 +1463,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="79.75"/>
-    <col customWidth="1" min="3" max="3" width="64.5"/>
-    <col customWidth="1" min="4" max="4" width="30.25"/>
-    <col customWidth="1" min="5" max="5" width="79.75"/>
+    <col min="2" max="2" width="79.6640625" customWidth="1"/>
+    <col min="3" max="3" width="64.5" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+    <col min="5" max="5" width="79.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1465,9 +1501,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>43657.0</v>
+        <v>43657</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -1479,9 +1515,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>40411.0</v>
+        <v>40411</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -1493,9 +1529,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>43681.0</v>
+        <v>43681</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -1507,9 +1543,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>46685.0</v>
+        <v>46685</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>13</v>
@@ -1521,9 +1557,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>40706.0</v>
+        <v>40706</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
@@ -1535,9 +1571,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>38854.0</v>
+        <v>38854</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>18</v>
@@ -1549,9 +1585,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>43859.0</v>
+        <v>43859</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>20</v>
@@ -1563,9 +1599,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>43344.0</v>
+        <v>43344</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>22</v>
@@ -1577,9 +1613,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <v>48233.0</v>
+        <v>48233</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>25</v>
@@ -1591,9 +1627,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
-        <v>39905.0</v>
+        <v>39905</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
@@ -1605,9 +1641,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <v>43581.0</v>
+        <v>43581</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>29</v>
@@ -1619,9 +1655,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <v>44292.0</v>
+        <v>44292</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>31</v>
@@ -1633,9 +1669,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <v>47467.0</v>
+        <v>47467</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>33</v>
@@ -1647,9 +1683,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <v>40836.0</v>
+        <v>40836</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>35</v>
@@ -1661,9 +1697,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>41337.0</v>
+        <v>41337</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>38</v>
@@ -1672,9 +1708,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <v>51021.0</v>
+        <v>51021</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>40</v>
@@ -1686,9 +1722,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <v>41431.0</v>
+        <v>41431</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>42</v>
@@ -1697,9 +1733,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <v>38522.0</v>
+        <v>38522</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>44</v>
@@ -1711,9 +1747,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
-        <v>39277.0</v>
+        <v>39277</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>46</v>
@@ -1725,9 +1761,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
-        <v>46456.0</v>
+        <v>46456</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>49</v>
@@ -1736,9 +1772,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
-        <v>40377.0</v>
+        <v>40377</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>51</v>
@@ -1750,9 +1786,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
-        <v>48451.0</v>
+        <v>48451</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>53</v>
@@ -1764,9 +1800,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
-        <v>50770.0</v>
+        <v>50770</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>55</v>
@@ -1778,9 +1814,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
-        <v>48051.0</v>
+        <v>48051</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>57</v>
@@ -1788,13 +1824,13 @@
       <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26">
+      <c r="D25" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
-        <v>50325.0</v>
+        <v>50325</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>59</v>
@@ -1806,9 +1842,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
-        <v>45305.0</v>
+        <v>45305</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>61</v>
@@ -1820,9 +1856,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
-        <v>50448.0</v>
+        <v>50448</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>63</v>
@@ -1834,9 +1870,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
-        <v>48912.0</v>
+        <v>48912</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>65</v>
@@ -1848,9 +1884,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
-        <v>52074.0</v>
+        <v>52074</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>67</v>
@@ -1862,9 +1898,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
-        <v>44135.0</v>
+        <v>44135</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>69</v>
@@ -1876,9 +1912,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
-        <v>50719.0</v>
+        <v>50719</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>71</v>
@@ -1890,9 +1926,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
-        <v>43490.0</v>
+        <v>43490</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>73</v>
@@ -1904,9 +1940,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
-        <v>40063.0</v>
+        <v>40063</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>75</v>
@@ -1918,9 +1954,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
-        <v>40539.0</v>
+        <v>40539</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>76</v>
@@ -1932,9 +1968,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
-        <v>45221.0</v>
+        <v>45221</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>78</v>
@@ -1946,9 +1982,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
-        <v>41549.0</v>
+        <v>41549</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>80</v>
@@ -1957,9 +1993,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
-        <v>50802.0</v>
+        <v>50802</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>82</v>
@@ -1971,9 +2007,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
-        <v>48487.0</v>
+        <v>48487</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>84</v>
@@ -1985,9 +2021,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
-        <v>42787.0</v>
+        <v>42787</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>87</v>
@@ -1999,9 +2035,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
-        <v>46528.0</v>
+        <v>46528</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>89</v>
@@ -2010,9 +2046,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
-        <v>40575.0</v>
+        <v>40575</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>91</v>
@@ -2024,9 +2060,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
-        <v>38688.0</v>
+        <v>38688</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>93</v>
@@ -2038,9 +2074,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
-        <v>42699.0</v>
+        <v>42699</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>95</v>
@@ -2052,9 +2088,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
-        <v>47461.0</v>
+        <v>47461</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>97</v>
@@ -2066,9 +2102,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1">
-        <v>41335.0</v>
+        <v>41335</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>100</v>
@@ -2077,9 +2113,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1">
-        <v>43653.0</v>
+        <v>43653</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>101</v>
@@ -2091,9 +2127,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
-        <v>41088.0</v>
+        <v>41088</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>103</v>
@@ -2102,9 +2138,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
-        <v>43453.0</v>
+        <v>43453</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>105</v>
@@ -2116,9 +2152,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
-        <v>44942.0</v>
+        <v>44942</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>107</v>
@@ -2130,9 +2166,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
-        <v>52424.0</v>
+        <v>52424</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>109</v>
@@ -2144,9 +2180,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
-        <v>38771.0</v>
+        <v>38771</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>111</v>
@@ -2158,9 +2194,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
-        <v>45271.0</v>
+        <v>45271</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>113</v>
@@ -2172,9 +2208,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
-        <v>47572.0</v>
+        <v>47572</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>114</v>
@@ -2186,9 +2222,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
-        <v>39842.0</v>
+        <v>39842</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>116</v>
@@ -2200,9 +2236,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
-        <v>40339.0</v>
+        <v>40339</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>118</v>
@@ -2214,9 +2250,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
-        <v>47976.0</v>
+        <v>47976</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>120</v>
@@ -2228,9 +2264,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="1">
-        <v>39759.0</v>
+        <v>39759</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>122</v>
@@ -2242,9 +2278,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="1">
-        <v>45420.0</v>
+        <v>45420</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>124</v>
@@ -2256,9 +2292,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="1">
-        <v>44443.0</v>
+        <v>44443</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>126</v>
@@ -2270,9 +2306,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="1">
-        <v>40817.0</v>
+        <v>40817</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>128</v>
@@ -2284,9 +2320,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="1">
-        <v>45729.0</v>
+        <v>45729</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>130</v>
@@ -2298,9 +2334,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="1">
-        <v>39264.0</v>
+        <v>39264</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>132</v>
@@ -2312,9 +2348,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="1">
-        <v>39372.0</v>
+        <v>39372</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>134</v>
@@ -2326,9 +2362,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="1">
-        <v>41617.0</v>
+        <v>41617</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>136</v>
@@ -2337,9 +2373,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="1">
-        <v>51861.0</v>
+        <v>51861</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>138</v>
@@ -2351,9 +2387,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
-        <v>42726.0</v>
+        <v>42726</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>140</v>
@@ -2365,9 +2401,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="1">
-        <v>47767.0</v>
+        <v>47767</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>142</v>
@@ -2379,9 +2415,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="1">
-        <v>48704.0</v>
+        <v>48704</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>144</v>
@@ -2389,13 +2425,13 @@
       <c r="C69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70">
+      <c r="D69" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="1">
-        <v>47334.0</v>
+        <v>47334</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>146</v>
@@ -2407,9 +2443,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="1">
-        <v>38571.0</v>
+        <v>38571</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>148</v>
@@ -2421,9 +2457,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="1">
-        <v>46026.0</v>
+        <v>46026</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>150</v>
@@ -2435,9 +2471,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="1">
-        <v>45811.0</v>
+        <v>45811</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>151</v>
@@ -2449,9 +2485,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="1">
-        <v>44011.0</v>
+        <v>44011</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>153</v>
@@ -2463,9 +2499,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
-        <v>45041.0</v>
+        <v>45041</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>155</v>
@@ -2477,9 +2513,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="1">
-        <v>39098.0</v>
+        <v>39098</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>157</v>
@@ -2491,9 +2527,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
-        <v>51051.0</v>
+        <v>51051</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>159</v>
@@ -2505,9 +2541,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
-        <v>45664.0</v>
+        <v>45664</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>160</v>
@@ -2516,9 +2552,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1">
-        <v>51131.0</v>
+        <v>51131</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>162</v>
@@ -2527,9 +2563,9 @@
         <v>163</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
-        <v>49462.0</v>
+        <v>49462</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>164</v>
@@ -2538,9 +2574,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
-        <v>50946.0</v>
+        <v>50946</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>166</v>
@@ -2552,9 +2588,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
-        <v>44769.0</v>
+        <v>44769</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>168</v>
@@ -2566,9 +2602,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
-        <v>46505.0</v>
+        <v>46505</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>169</v>
@@ -2577,9 +2613,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
-        <v>46740.0</v>
+        <v>46740</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>171</v>
@@ -2588,9 +2624,9 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
-        <v>40548.0</v>
+        <v>40548</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>173</v>
@@ -2602,9 +2638,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
-        <v>44079.0</v>
+        <v>44079</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>175</v>
@@ -2613,9 +2649,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
-        <v>39915.0</v>
+        <v>39915</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>177</v>
@@ -2627,9 +2663,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
-        <v>44929.0</v>
+        <v>44929</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>179</v>
@@ -2641,9 +2677,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
-        <v>43587.0</v>
+        <v>43587</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>180</v>
@@ -2655,9 +2691,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
-        <v>47848.0</v>
+        <v>47848</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>182</v>
@@ -2666,9 +2702,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
-        <v>48147.0</v>
+        <v>48147</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>184</v>
@@ -2680,9 +2716,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
-        <v>45851.0</v>
+        <v>45851</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>186</v>
@@ -2690,13 +2726,13 @@
       <c r="C92" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="93">
+      <c r="D92" s="4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
-        <v>49323.0</v>
+        <v>49323</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>188</v>
@@ -2708,9 +2744,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
-        <v>52559.0</v>
+        <v>52559</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>190</v>
@@ -2722,9 +2758,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
-        <v>43392.0</v>
+        <v>43392</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>192</v>
@@ -2736,9 +2772,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
-        <v>49998.0</v>
+        <v>49998</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>194</v>
@@ -2747,9 +2783,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
-        <v>44747.0</v>
+        <v>44747</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>195</v>
@@ -2758,9 +2794,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
-        <v>44572.0</v>
+        <v>44572</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>197</v>
@@ -2769,9 +2805,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
-        <v>40970.0</v>
+        <v>40970</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>199</v>
@@ -2780,9 +2816,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
-        <v>40139.0</v>
+        <v>40139</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>201</v>
@@ -2791,9 +2827,9 @@
         <v>202</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
-        <v>53166.0</v>
+        <v>53166</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>203</v>
@@ -2805,9 +2841,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
-        <v>39888.0</v>
+        <v>39888</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>205</v>
@@ -2819,9 +2855,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
-        <v>51007.0</v>
+        <v>51007</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>206</v>
@@ -2833,9 +2869,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
-        <v>38954.0</v>
+        <v>38954</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>208</v>
@@ -2847,9 +2883,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
-        <v>42733.0</v>
+        <v>42733</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>210</v>
@@ -2861,9 +2897,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="1">
-        <v>40684.0</v>
+        <v>40684</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>212</v>
@@ -2875,9 +2911,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="1">
-        <v>47697.0</v>
+        <v>47697</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>214</v>
@@ -2889,9 +2925,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="1">
-        <v>47560.0</v>
+        <v>47560</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>216</v>
@@ -2903,9 +2939,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="1">
-        <v>39760.0</v>
+        <v>39760</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>218</v>
@@ -2917,9 +2953,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="1">
-        <v>41748.0</v>
+        <v>41748</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>220</v>
@@ -2931,9 +2967,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="1">
-        <v>48194.0</v>
+        <v>48194</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>222</v>
@@ -2942,9 +2978,9 @@
         <v>223</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="1">
-        <v>41815.0</v>
+        <v>41815</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>224</v>
@@ -2956,9 +2992,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="1">
-        <v>41839.0</v>
+        <v>41839</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>226</v>
@@ -2970,9 +3006,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="1">
-        <v>43804.0</v>
+        <v>43804</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>227</v>
@@ -2984,9 +3020,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="1">
-        <v>49959.0</v>
+        <v>49959</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>229</v>
@@ -2998,9 +3034,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="1">
-        <v>50643.0</v>
+        <v>50643</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>231</v>
@@ -3012,9 +3048,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="1">
-        <v>45773.0</v>
+        <v>45773</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>233</v>
@@ -3026,9 +3062,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="1">
-        <v>43422.0</v>
+        <v>43422</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>235</v>
@@ -3040,9 +3076,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="1">
-        <v>45817.0</v>
+        <v>45817</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>237</v>
@@ -3054,9 +3090,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="1">
-        <v>40053.0</v>
+        <v>40053</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>239</v>
@@ -3068,9 +3104,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="1">
-        <v>42731.0</v>
+        <v>42731</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>241</v>
@@ -3082,9 +3118,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="1">
-        <v>46428.0</v>
+        <v>46428</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>243</v>
@@ -3096,9 +3132,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="1">
-        <v>41122.0</v>
+        <v>41122</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>245</v>
@@ -3107,9 +3143,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="1">
-        <v>41608.0</v>
+        <v>41608</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>247</v>
@@ -3118,9 +3154,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="1">
-        <v>47702.0</v>
+        <v>47702</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>248</v>
@@ -3132,9 +3168,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="1">
-        <v>40310.0</v>
+        <v>40310</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>250</v>
@@ -3146,9 +3182,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="1">
-        <v>46582.0</v>
+        <v>46582</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>252</v>
@@ -3157,9 +3193,9 @@
         <v>253</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="1">
-        <v>40067.0</v>
+        <v>40067</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>254</v>
@@ -3171,9 +3207,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="1">
-        <v>44763.0</v>
+        <v>44763</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>256</v>
@@ -3185,9 +3221,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="1">
-        <v>43540.0</v>
+        <v>43540</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>258</v>
@@ -3199,9 +3235,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="1">
-        <v>44285.0</v>
+        <v>44285</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>260</v>
@@ -3210,9 +3246,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="1">
-        <v>41487.0</v>
+        <v>41487</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>262</v>
@@ -3221,9 +3257,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="1">
-        <v>40258.0</v>
+        <v>40258</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>263</v>
@@ -3235,9 +3271,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="1">
-        <v>38684.0</v>
+        <v>38684</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>264</v>
@@ -3249,9 +3285,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="1">
-        <v>42719.0</v>
+        <v>42719</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>266</v>
@@ -3263,9 +3299,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="1">
-        <v>46426.0</v>
+        <v>46426</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>268</v>
@@ -3277,9 +3313,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="1">
-        <v>38790.0</v>
+        <v>38790</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>270</v>
@@ -3291,9 +3327,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="1">
-        <v>39382.0</v>
+        <v>39382</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>272</v>
@@ -3305,9 +3341,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="1">
-        <v>41300.0</v>
+        <v>41300</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>274</v>
@@ -3316,9 +3352,9 @@
         <v>275</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="1">
-        <v>44950.0</v>
+        <v>44950</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>276</v>
@@ -3330,9 +3366,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="1">
-        <v>43277.0</v>
+        <v>43277</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>277</v>
@@ -3344,9 +3380,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="1">
-        <v>43520.0</v>
+        <v>43520</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>278</v>
@@ -3358,9 +3394,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="1">
-        <v>43666.0</v>
+        <v>43666</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>280</v>
@@ -3372,9 +3408,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="1">
-        <v>48327.0</v>
+        <v>48327</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>282</v>
@@ -3386,20 +3422,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="1">
-        <v>47819.0</v>
+        <v>47819</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C145" s="1">
-        <v>395.0</v>
-      </c>
-    </row>
-    <row r="146">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="1">
-        <v>46762.0</v>
+        <v>46762</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>285</v>
@@ -3411,9 +3447,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="1">
-        <v>45694.0</v>
+        <v>45694</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>287</v>
@@ -3425,9 +3461,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="1">
-        <v>50929.0</v>
+        <v>50929</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>289</v>
@@ -3439,9 +3475,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A149" s="1">
-        <v>48542.0</v>
+        <v>48542</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>290</v>
@@ -3450,9 +3486,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="1">
-        <v>48431.0</v>
+        <v>48431</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>292</v>
@@ -3464,9 +3500,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="1">
-        <v>41304.0</v>
+        <v>41304</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>294</v>
@@ -3475,9 +3511,9 @@
         <v>295</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A152" s="1">
-        <v>52971.0</v>
+        <v>52971</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>296</v>
@@ -3489,9 +3525,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="1">
-        <v>48663.0</v>
+        <v>48663</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>297</v>
@@ -3503,9 +3539,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="1">
-        <v>44283.0</v>
+        <v>44283</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>299</v>
@@ -3514,9 +3550,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A155" s="1">
-        <v>45231.0</v>
+        <v>45231</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>301</v>
@@ -3528,9 +3564,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="1">
-        <v>45040.0</v>
+        <v>45040</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>302</v>
@@ -3542,9 +3578,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="1">
-        <v>40646.0</v>
+        <v>40646</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>304</v>
@@ -3556,9 +3592,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="1">
-        <v>39897.0</v>
+        <v>39897</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>306</v>
@@ -3570,9 +3606,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="1">
-        <v>48554.0</v>
+        <v>48554</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>308</v>
@@ -3584,9 +3620,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="1">
-        <v>45286.0</v>
+        <v>45286</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>310</v>
@@ -3595,9 +3631,9 @@
         <v>311</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="1">
-        <v>41103.0</v>
+        <v>41103</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>312</v>
@@ -3606,9 +3642,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="1">
-        <v>49085.0</v>
+        <v>49085</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>313</v>
@@ -3617,9 +3653,9 @@
         <v>314</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="1">
-        <v>43790.0</v>
+        <v>43790</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>315</v>
@@ -3628,9 +3664,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="1">
-        <v>43970.0</v>
+        <v>43970</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>317</v>
@@ -3639,9 +3675,9 @@
         <v>318</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="1">
-        <v>47570.0</v>
+        <v>47570</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>319</v>
@@ -3650,9 +3686,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="1">
-        <v>47152.0</v>
+        <v>47152</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>320</v>
@@ -3661,9 +3697,9 @@
         <v>321</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="1">
-        <v>40202.0</v>
+        <v>40202</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>322</v>
@@ -3672,9 +3708,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="1">
-        <v>45603.0</v>
+        <v>45603</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>323</v>
@@ -3683,9 +3719,9 @@
         <v>324</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="1">
-        <v>40076.0</v>
+        <v>40076</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>325</v>
@@ -3694,9 +3730,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A170" s="1">
-        <v>52567.0</v>
+        <v>52567</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>327</v>
@@ -3705,9 +3741,9 @@
         <v>328</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="1">
-        <v>38582.0</v>
+        <v>38582</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>329</v>
@@ -3716,9 +3752,9 @@
         <v>330</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="1">
-        <v>48112.0</v>
+        <v>48112</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>331</v>
@@ -3727,9 +3763,9 @@
         <v>332</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="1">
-        <v>47135.0</v>
+        <v>47135</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>333</v>
@@ -3738,9 +3774,9 @@
         <v>334</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="1">
-        <v>39181.0</v>
+        <v>39181</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>335</v>
@@ -3749,9 +3785,9 @@
         <v>336</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="1">
-        <v>46487.0</v>
+        <v>46487</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>337</v>
@@ -3760,9 +3796,9 @@
         <v>338</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="1">
-        <v>51265.0</v>
+        <v>51265</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>339</v>
@@ -3771,9 +3807,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="1">
-        <v>45011.0</v>
+        <v>45011</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>340</v>
@@ -3782,9 +3818,9 @@
         <v>341</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="1">
-        <v>51117.0</v>
+        <v>51117</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>342</v>
@@ -3793,9 +3829,9 @@
         <v>343</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="1">
-        <v>50604.0</v>
+        <v>50604</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>344</v>
@@ -3804,9 +3840,9 @@
         <v>345</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="1">
-        <v>48077.0</v>
+        <v>48077</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>346</v>
@@ -3815,9 +3851,9 @@
         <v>347</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="1">
-        <v>51112.0</v>
+        <v>51112</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>348</v>
@@ -3826,9 +3862,9 @@
         <v>349</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A182" s="1">
-        <v>48675.0</v>
+        <v>48675</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>350</v>
@@ -3837,9 +3873,9 @@
         <v>351</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="1">
-        <v>50463.0</v>
+        <v>50463</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>352</v>
@@ -3848,9 +3884,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="1">
-        <v>47206.0</v>
+        <v>47206</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>354</v>
@@ -3859,9 +3895,9 @@
         <v>355</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="1">
-        <v>41573.0</v>
+        <v>41573</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>356</v>
@@ -3870,9 +3906,9 @@
         <v>357</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="1">
-        <v>49893.0</v>
+        <v>49893</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>358</v>
@@ -3881,9 +3917,9 @@
         <v>359</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="1">
-        <v>46928.0</v>
+        <v>46928</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>360</v>
@@ -3892,9 +3928,9 @@
         <v>361</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="1">
-        <v>46535.0</v>
+        <v>46535</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>362</v>
@@ -3903,9 +3939,9 @@
         <v>363</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="1">
-        <v>50417.0</v>
+        <v>50417</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>364</v>
@@ -3914,9 +3950,9 @@
         <v>365</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A190" s="1">
-        <v>38741.0</v>
+        <v>38741</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>366</v>
@@ -3925,9 +3961,9 @@
         <v>367</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="1">
-        <v>51234.0</v>
+        <v>51234</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>368</v>
@@ -3936,9 +3972,9 @@
         <v>369</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="1">
-        <v>39896.0</v>
+        <v>39896</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>370</v>
@@ -3947,9 +3983,9 @@
         <v>371</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="1">
-        <v>47848.0</v>
+        <v>47848</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>182</v>
@@ -3958,9 +3994,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A194" s="1">
-        <v>52754.0</v>
+        <v>52754</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>372</v>
@@ -3969,9 +4005,9 @@
         <v>373</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A195" s="1">
-        <v>47256.0</v>
+        <v>47256</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>374</v>
@@ -3980,9 +4016,9 @@
         <v>375</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="1">
-        <v>47331.0</v>
+        <v>47331</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>376</v>
@@ -3991,9 +4027,9 @@
         <v>377</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A197" s="1">
-        <v>46429.0</v>
+        <v>46429</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>378</v>
@@ -4002,9 +4038,9 @@
         <v>379</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A198" s="1">
-        <v>38731.0</v>
+        <v>38731</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>380</v>
@@ -4013,9 +4049,9 @@
         <v>381</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="1">
-        <v>44957.0</v>
+        <v>44957</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>382</v>
@@ -4024,9 +4060,9 @@
         <v>383</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A200" s="1">
-        <v>45360.0</v>
+        <v>45360</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>384</v>
@@ -4035,9 +4071,9 @@
         <v>385</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A201" s="1">
-        <v>45111.0</v>
+        <v>45111</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>386</v>
@@ -4048,197 +4084,197 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
-    <hyperlink r:id="rId7" ref="B8"/>
-    <hyperlink r:id="rId8" ref="B9"/>
-    <hyperlink r:id="rId9" ref="B10"/>
-    <hyperlink r:id="rId10" ref="B11"/>
-    <hyperlink r:id="rId11" ref="B12"/>
-    <hyperlink r:id="rId12" ref="B13"/>
-    <hyperlink r:id="rId13" ref="B14"/>
-    <hyperlink r:id="rId14" ref="B15"/>
-    <hyperlink r:id="rId15" ref="B16"/>
-    <hyperlink r:id="rId16" ref="B17"/>
-    <hyperlink r:id="rId17" ref="B18"/>
-    <hyperlink r:id="rId18" ref="B19"/>
-    <hyperlink r:id="rId19" ref="B20"/>
-    <hyperlink r:id="rId20" ref="B21"/>
-    <hyperlink r:id="rId21" ref="B22"/>
-    <hyperlink r:id="rId22" ref="B23"/>
-    <hyperlink r:id="rId23" ref="B24"/>
-    <hyperlink r:id="rId24" ref="B25"/>
-    <hyperlink r:id="rId25" ref="B26"/>
-    <hyperlink r:id="rId26" ref="B27"/>
-    <hyperlink r:id="rId27" ref="B28"/>
-    <hyperlink r:id="rId28" ref="B29"/>
-    <hyperlink r:id="rId29" ref="B30"/>
-    <hyperlink r:id="rId30" ref="B31"/>
-    <hyperlink r:id="rId31" ref="B32"/>
-    <hyperlink r:id="rId32" ref="B33"/>
-    <hyperlink r:id="rId33" ref="B34"/>
-    <hyperlink r:id="rId34" ref="B35"/>
-    <hyperlink r:id="rId35" ref="B36"/>
-    <hyperlink r:id="rId36" ref="B37"/>
-    <hyperlink r:id="rId37" ref="B38"/>
-    <hyperlink r:id="rId38" ref="B40"/>
-    <hyperlink r:id="rId39" ref="B41"/>
-    <hyperlink r:id="rId40" ref="B42"/>
-    <hyperlink r:id="rId41" ref="B43"/>
-    <hyperlink r:id="rId42" ref="B44"/>
-    <hyperlink r:id="rId43" ref="B45"/>
-    <hyperlink r:id="rId44" ref="B46"/>
-    <hyperlink r:id="rId45" ref="B47"/>
-    <hyperlink r:id="rId46" ref="B48"/>
-    <hyperlink r:id="rId47" ref="B49"/>
-    <hyperlink r:id="rId48" ref="B50"/>
-    <hyperlink r:id="rId49" ref="B51"/>
-    <hyperlink r:id="rId50" ref="B52"/>
-    <hyperlink r:id="rId51" ref="B53"/>
-    <hyperlink r:id="rId52" ref="B54"/>
-    <hyperlink r:id="rId53" ref="B55"/>
-    <hyperlink r:id="rId54" ref="B56"/>
-    <hyperlink r:id="rId55" ref="B57"/>
-    <hyperlink r:id="rId56" ref="B58"/>
-    <hyperlink r:id="rId57" ref="B59"/>
-    <hyperlink r:id="rId58" ref="B60"/>
-    <hyperlink r:id="rId59" ref="B61"/>
-    <hyperlink r:id="rId60" ref="B62"/>
-    <hyperlink r:id="rId61" ref="B63"/>
-    <hyperlink r:id="rId62" ref="B64"/>
-    <hyperlink r:id="rId63" ref="B65"/>
-    <hyperlink r:id="rId64" ref="B66"/>
-    <hyperlink r:id="rId65" ref="B67"/>
-    <hyperlink r:id="rId66" ref="B69"/>
-    <hyperlink r:id="rId67" ref="B70"/>
-    <hyperlink r:id="rId68" ref="B71"/>
-    <hyperlink r:id="rId69" ref="B72"/>
-    <hyperlink r:id="rId70" ref="B73"/>
-    <hyperlink r:id="rId71" ref="B74"/>
-    <hyperlink r:id="rId72" ref="B75"/>
-    <hyperlink r:id="rId73" ref="B76"/>
-    <hyperlink r:id="rId74" ref="B77"/>
-    <hyperlink r:id="rId75" ref="B78"/>
-    <hyperlink r:id="rId76" ref="B79"/>
-    <hyperlink r:id="rId77" ref="B80"/>
-    <hyperlink r:id="rId78" ref="B81"/>
-    <hyperlink r:id="rId79" ref="B82"/>
-    <hyperlink r:id="rId80" ref="B83"/>
-    <hyperlink r:id="rId81" ref="B84"/>
-    <hyperlink r:id="rId82" ref="B85"/>
-    <hyperlink r:id="rId83" ref="B86"/>
-    <hyperlink r:id="rId84" ref="B87"/>
-    <hyperlink r:id="rId85" ref="B88"/>
-    <hyperlink r:id="rId86" ref="B89"/>
-    <hyperlink r:id="rId87" ref="B90"/>
-    <hyperlink r:id="rId88" ref="B91"/>
-    <hyperlink r:id="rId89" ref="B92"/>
-    <hyperlink r:id="rId90" ref="B93"/>
-    <hyperlink r:id="rId91" ref="B94"/>
-    <hyperlink r:id="rId92" ref="B95"/>
-    <hyperlink r:id="rId93" ref="B97"/>
-    <hyperlink r:id="rId94" ref="B98"/>
-    <hyperlink r:id="rId95" ref="B99"/>
-    <hyperlink r:id="rId96" ref="B100"/>
-    <hyperlink r:id="rId97" ref="B101"/>
-    <hyperlink r:id="rId98" ref="B102"/>
-    <hyperlink r:id="rId99" ref="B103"/>
-    <hyperlink r:id="rId100" ref="B104"/>
-    <hyperlink r:id="rId101" ref="B105"/>
-    <hyperlink r:id="rId102" ref="B106"/>
-    <hyperlink r:id="rId103" ref="B107"/>
-    <hyperlink r:id="rId104" ref="B109"/>
-    <hyperlink r:id="rId105" ref="B110"/>
-    <hyperlink r:id="rId106" ref="B111"/>
-    <hyperlink r:id="rId107" ref="B112"/>
-    <hyperlink r:id="rId108" ref="B113"/>
-    <hyperlink r:id="rId109" ref="B114"/>
-    <hyperlink r:id="rId110" ref="B115"/>
-    <hyperlink r:id="rId111" ref="B116"/>
-    <hyperlink r:id="rId112" ref="B117"/>
-    <hyperlink r:id="rId113" ref="B118"/>
-    <hyperlink r:id="rId114" ref="B119"/>
-    <hyperlink r:id="rId115" ref="B120"/>
-    <hyperlink r:id="rId116" ref="B121"/>
-    <hyperlink r:id="rId117" ref="B122"/>
-    <hyperlink r:id="rId118" ref="B123"/>
-    <hyperlink r:id="rId119" ref="B124"/>
-    <hyperlink r:id="rId120" ref="B126"/>
-    <hyperlink r:id="rId121" ref="B127"/>
-    <hyperlink r:id="rId122" ref="B128"/>
-    <hyperlink r:id="rId123" ref="B129"/>
-    <hyperlink r:id="rId124" ref="B130"/>
-    <hyperlink r:id="rId125" ref="B131"/>
-    <hyperlink r:id="rId126" ref="B132"/>
-    <hyperlink r:id="rId127" ref="B133"/>
-    <hyperlink r:id="rId128" ref="B134"/>
-    <hyperlink r:id="rId129" ref="B135"/>
-    <hyperlink r:id="rId130" ref="B136"/>
-    <hyperlink r:id="rId131" ref="B137"/>
-    <hyperlink r:id="rId132" ref="B138"/>
-    <hyperlink r:id="rId133" ref="B139"/>
-    <hyperlink r:id="rId134" ref="B140"/>
-    <hyperlink r:id="rId135" ref="B141"/>
-    <hyperlink r:id="rId136" ref="B142"/>
-    <hyperlink r:id="rId137" ref="B143"/>
-    <hyperlink r:id="rId138" ref="B145"/>
-    <hyperlink r:id="rId139" ref="B146"/>
-    <hyperlink r:id="rId140" ref="B147"/>
-    <hyperlink r:id="rId141" ref="B148"/>
-    <hyperlink r:id="rId142" ref="B149"/>
-    <hyperlink r:id="rId143" ref="B151"/>
-    <hyperlink r:id="rId144" ref="B152"/>
-    <hyperlink r:id="rId145" ref="B153"/>
-    <hyperlink r:id="rId146" ref="B154"/>
-    <hyperlink r:id="rId147" ref="B155"/>
-    <hyperlink r:id="rId148" ref="B156"/>
-    <hyperlink r:id="rId149" ref="B157"/>
-    <hyperlink r:id="rId150" ref="B158"/>
-    <hyperlink r:id="rId151" ref="B160"/>
-    <hyperlink r:id="rId152" ref="B161"/>
-    <hyperlink r:id="rId153" ref="B162"/>
-    <hyperlink r:id="rId154" ref="B163"/>
-    <hyperlink r:id="rId155" ref="B164"/>
-    <hyperlink r:id="rId156" ref="B165"/>
-    <hyperlink r:id="rId157" ref="B166"/>
-    <hyperlink r:id="rId158" ref="B167"/>
-    <hyperlink r:id="rId159" ref="B168"/>
-    <hyperlink r:id="rId160" ref="B169"/>
-    <hyperlink r:id="rId161" ref="B170"/>
-    <hyperlink r:id="rId162" ref="B171"/>
-    <hyperlink r:id="rId163" ref="B172"/>
-    <hyperlink r:id="rId164" ref="B173"/>
-    <hyperlink r:id="rId165" ref="B174"/>
-    <hyperlink r:id="rId166" ref="B175"/>
-    <hyperlink r:id="rId167" ref="B176"/>
-    <hyperlink r:id="rId168" ref="B177"/>
-    <hyperlink r:id="rId169" ref="B178"/>
-    <hyperlink r:id="rId170" ref="B179"/>
-    <hyperlink r:id="rId171" ref="B180"/>
-    <hyperlink r:id="rId172" ref="B181"/>
-    <hyperlink r:id="rId173" ref="B182"/>
-    <hyperlink r:id="rId174" ref="B183"/>
-    <hyperlink r:id="rId175" ref="B185"/>
-    <hyperlink r:id="rId176" ref="B186"/>
-    <hyperlink r:id="rId177" ref="B187"/>
-    <hyperlink r:id="rId178" ref="B188"/>
-    <hyperlink r:id="rId179" ref="B189"/>
-    <hyperlink r:id="rId180" ref="B190"/>
-    <hyperlink r:id="rId181" ref="B191"/>
-    <hyperlink r:id="rId182" ref="B192"/>
-    <hyperlink r:id="rId183" ref="B193"/>
-    <hyperlink r:id="rId184" ref="B194"/>
-    <hyperlink r:id="rId185" ref="B196"/>
-    <hyperlink r:id="rId186" ref="B197"/>
-    <hyperlink r:id="rId187" ref="B198"/>
-    <hyperlink r:id="rId188" ref="B199"/>
-    <hyperlink r:id="rId189" ref="B200"/>
-    <hyperlink r:id="rId190" ref="B201"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B70" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B71" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B72" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B73" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B74" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B75" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B76" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B77" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B78" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B79" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B80" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B81" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B82" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B83" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B84" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B85" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B86" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B87" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B93" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B94" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B95" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B97" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B98" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B99" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B100" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B101" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B102" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B103" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B104" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B105" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B106" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B107" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B109" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B110" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B111" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B112" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B113" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B114" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B115" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B116" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B117" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B118" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B119" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B120" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B121" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B122" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B123" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B124" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B126" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B127" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B128" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B129" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B130" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B131" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B132" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B133" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B134" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B135" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B136" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B137" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B138" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B139" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B140" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B141" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B142" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B143" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="B145" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B146" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="B147" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B148" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="B149" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B151" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="B152" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B153" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="B154" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B155" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="B156" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B157" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="B158" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B160" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="B161" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="B162" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="B163" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="B164" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="B165" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="B166" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="B167" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="B168" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="B169" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="B170" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="B171" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B172" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="B173" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B174" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="B175" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="B176" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="B177" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B178" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="B179" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B180" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="B181" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="B182" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="B183" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="B185" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="B186" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="B187" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="B188" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="B189" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="B190" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="B191" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="B192" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="B193" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="B194" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="B196" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="B197" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="B198" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="B199" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="B200" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="B201" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
   </hyperlinks>
-  <drawing r:id="rId191"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>